<commit_message>
Add second field to test form
</commit_message>
<xml_diff>
--- a/extras/test-form/Plug-in test form - clickable-svg.xlsx
+++ b/extras/test-form/Plug-in test form - clickable-svg.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7733" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11870" uniqueCount="411">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2761,6 +2761,15 @@
   </si>
   <si>
     <t>custom-example-svg-imagemap</t>
+  </si>
+  <si>
+    <t>continent</t>
+  </si>
+  <si>
+    <t>On which continent do you live?</t>
+  </si>
+  <si>
+    <t>map of the world.svg</t>
   </si>
 </sst>
 </file>
@@ -6532,16 +6541,16 @@
     </row>
     <row r="12" spans="1:23" ht="306" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>380</v>
+        <v>99</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>380</v>
+        <v>408</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>380</v>
+        <v>409</v>
       </c>
       <c r="F12" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>380</v>
@@ -6550,10 +6559,10 @@
         <v>380</v>
       </c>
       <c r="K12" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="P12" t="s">
-        <v>380</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="34" x14ac:dyDescent="0.2">
@@ -6882,7 +6891,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f>TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003051654</v>
+        <v>2003101636</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>380</v>

</xml_diff>